<commit_message>
Output to user selected folder
</commit_message>
<xml_diff>
--- a/ExportedData/SingleTag_1.xlsx
+++ b/ExportedData/SingleTag_1.xlsx
@@ -33,7 +33,7 @@
     <t>C0045392F</t>
   </si>
   <si>
-    <t>2020-11-09</t>
+    <t>2020-11-10</t>
   </si>
   <si>
     <t>/Users/Keshab/Desktop/AllImages/1.jpg</t>
@@ -491,7 +491,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -547,7 +547,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>

</xml_diff>